<commit_message>
updated example files to include inputs for RPS and capacity credits. These constraints only work with the stochastic version of temoa that is included in this repo
</commit_message>
<xml_diff>
--- a/examples/baselines/data/scenarios.xlsx
+++ b/examples/baselines/data/scenarios.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6C295C2-F7A3-4C4E-826D-65C8F257A991}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{140B3396-53B1-4928-A484-9A2ECBC2E437}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SolverSettings" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="65">
   <si>
     <t>Scenario</t>
   </si>
@@ -215,6 +215,9 @@
   </si>
   <si>
     <t>F</t>
+  </si>
+  <si>
+    <t>include_RPS</t>
   </si>
 </sst>
 </file>
@@ -534,10 +537,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:AA1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -751,6 +754,29 @@
       </c>
       <c r="G9">
         <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G10" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1478,7 +1504,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>